<commit_message>
Estadisticas de Cliente version final
</commit_message>
<xml_diff>
--- a/reportes/base/oestadisticasCliente.xlsx
+++ b/reportes/base/oestadisticasCliente.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920D5224-93D0-4904-9594-21B4AE271F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF8F7FF-78FD-492D-B15A-2CBB3DFC23FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +110,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -242,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -267,37 +260,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,7 +606,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="145" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,20 +622,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="21">
+      <c r="H1" s="13">
         <f ca="1">TODAY()</f>
-        <v>44780</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -662,31 +652,31 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="15" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -725,7 +715,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1081,15 +1071,15 @@
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>